<commit_message>
Corrección y primera auditoría
Se corrige el build plan para la primera iteración y se realiza la
primera auditoría respecto a lo implementado.
</commit_message>
<xml_diff>
--- a/Documentos/1. INICIO/INI-MNG-Anexo3AplicaciónDefiniciónMétricas-v1.0.xlsx
+++ b/Documentos/1. INICIO/INI-MNG-Anexo3AplicaciónDefiniciónMétricas-v1.0.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander Vargas\Google Drive\Ingeniería de Software 3\Proyecto Final\Entregas\02\Andrés_Montoya_Higgor_Vargas_SegundaEntrega\MeasurementPlan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14415" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Definición de métricas" sheetId="1" r:id="rId1"/>
     <sheet name="Aplicación de métricas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1001,9 +996,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1015,8 +1019,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1026,30 +1054,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1067,9 +1071,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1088,18 +1089,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="206">
-    <cellStyle name="Buena" xfId="77" builtinId="26"/>
+    <cellStyle name="Correcto" xfId="77" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1647,33 +1642,33 @@
       <selection activeCell="C4" sqref="C4:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="2" max="2" width="33.125" customWidth="1"/>
-    <col min="3" max="3" width="63.375" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1683,8 +1678,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+    <row r="4" spans="1:3">
+      <c r="A4" s="28"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1692,8 +1687,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:3">
+      <c r="A5" s="28"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1701,8 +1696,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1712,8 +1707,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+    <row r="7" spans="1:3">
+      <c r="A7" s="28"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1721,8 +1716,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+    <row r="8" spans="1:3">
+      <c r="A8" s="28"/>
       <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1730,8 +1725,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1741,8 +1736,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+    <row r="10" spans="1:3">
+      <c r="A10" s="28"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1750,8 +1745,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1761,8 +1756,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+    <row r="12" spans="1:3">
+      <c r="A12" s="28"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1770,8 +1765,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+    <row r="13" spans="1:3">
+      <c r="A13" s="28"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1779,8 +1774,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+    <row r="14" spans="1:3">
+      <c r="A14" s="28"/>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1788,8 +1783,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+    <row r="15" spans="1:3">
+      <c r="A15" s="28"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1797,8 +1792,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+    <row r="16" spans="1:3">
+      <c r="A16" s="28"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1806,8 +1801,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1817,8 +1812,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+    <row r="18" spans="1:3">
+      <c r="A18" s="28"/>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1826,8 +1821,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+    <row r="19" spans="1:3">
+      <c r="A19" s="28"/>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1835,8 +1830,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+    <row r="20" spans="1:3">
+      <c r="A20" s="28"/>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
@@ -1844,8 +1839,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="28" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1855,8 +1850,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+    <row r="22" spans="1:3">
+      <c r="A22" s="28"/>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1864,8 +1859,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+    <row r="23" spans="1:3">
+      <c r="A23" s="28"/>
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1873,8 +1868,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+    <row r="24" spans="1:3">
+      <c r="A24" s="28"/>
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1882,8 +1877,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+    <row r="25" spans="1:3">
+      <c r="A25" s="28"/>
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1891,8 +1886,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1902,8 +1897,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+    <row r="27" spans="1:3">
+      <c r="A27" s="28"/>
       <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1911,8 +1906,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+    <row r="28" spans="1:3">
+      <c r="A28" s="28"/>
       <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1920,8 +1915,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+    <row r="29" spans="1:3">
+      <c r="A29" s="28"/>
       <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1929,8 +1924,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
+    <row r="30" spans="1:3">
+      <c r="A30" s="28"/>
       <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1938,8 +1933,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1949,8 +1944,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+    <row r="32" spans="1:3">
+      <c r="A32" s="28"/>
       <c r="B32" s="1" t="s">
         <v>35</v>
       </c>
@@ -1958,8 +1953,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+    <row r="33" spans="1:3">
+      <c r="A33" s="28"/>
       <c r="B33" s="1" t="s">
         <v>36</v>
       </c>
@@ -1981,7 +1976,6 @@
     <mergeCell ref="A21:A25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1994,25 +1988,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3:J4"/>
+      <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="37.125" customWidth="1"/>
-    <col min="6" max="6" width="66.375" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" customWidth="1"/>
+    <col min="6" max="6" width="66.33203125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="11" width="17.625" style="23" customWidth="1"/>
+    <col min="9" max="11" width="17.6640625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="69" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>57</v>
       </c>
@@ -2038,25 +2032,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="32.25" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="44">
         <v>0.2</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="29">
         <f>K6</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="36">
+        <v>0.21660999999999997</v>
+      </c>
+      <c r="D2" s="29">
         <f>B2*C2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+        <v>4.3321999999999999E-2</v>
+      </c>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
       <c r="I2" s="22" t="s">
         <v>63</v>
       </c>
@@ -2067,52 +2061,54 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:11">
+      <c r="A3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="50" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="37">
         <v>0.7</v>
       </c>
-      <c r="J3" s="44"/>
-      <c r="K3" s="43">
+      <c r="J3" s="47">
+        <v>0.1666</v>
+      </c>
+      <c r="K3" s="37">
         <f>I3*J3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="43"/>
-    </row>
-    <row r="5" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+        <v>0.11661999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="43" customHeight="1">
+      <c r="A4" s="42"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="37"/>
+    </row>
+    <row r="5" spans="1:11" ht="45" customHeight="1">
+      <c r="A5" s="42"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="15" t="s">
         <v>1</v>
       </c>
@@ -2128,23 +2124,25 @@
       <c r="I5" s="5">
         <v>0.3</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="25">
+        <v>0.33329999999999999</v>
+      </c>
       <c r="K5" s="5">
         <f>I5*J5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="45" t="s">
+        <v>9.9989999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" customHeight="1">
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="50"/>
       <c r="I6" s="5">
         <f>SUM(I3:I5)</f>
         <v>1</v>
@@ -2152,28 +2150,28 @@
       <c r="J6" s="25"/>
       <c r="K6" s="5">
         <f>SUM(K3:K5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.21660999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="32" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="44">
         <v>0.1</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="29">
         <f>K11</f>
         <v>0</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="29">
         <f>B7*C7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="22" t="s">
         <v>63</v>
       </c>
@@ -2184,13 +2182,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:11" ht="58" customHeight="1">
+      <c r="A8" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="15" t="s">
         <v>4</v>
       </c>
@@ -2212,11 +2210,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+    <row r="9" spans="1:11" ht="42" customHeight="1">
+      <c r="A9" s="42"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="15" t="s">
         <v>5</v>
       </c>
@@ -2238,11 +2236,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+    <row r="10" spans="1:11" ht="46" customHeight="1">
+      <c r="A10" s="42"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="15" t="s">
         <v>39</v>
       </c>
@@ -2264,17 +2262,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="40" t="s">
+    <row r="11" spans="1:11" ht="20" customHeight="1">
+      <c r="A11" s="43"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="5">
         <f>SUM(I8:I10)</f>
         <v>1</v>
@@ -2285,25 +2283,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="31" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="38">
         <v>0.15</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="29">
         <f>K14</f>
         <v>0</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="29">
         <f>B12*C12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="56"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
       <c r="I12" s="22" t="s">
         <v>63</v>
       </c>
@@ -2314,13 +2312,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:11" ht="45" customHeight="1">
+      <c r="A13" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="15" t="s">
         <v>8</v>
       </c>
@@ -2342,17 +2340,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="40" t="s">
+    <row r="14" spans="1:11" ht="17" customHeight="1">
+      <c r="A14" s="34"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="5">
         <f>I13</f>
         <v>1</v>
@@ -2363,25 +2361,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="33" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="38">
         <v>0.15</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="29">
         <f>K20</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="36">
+        <v>0.13331999999999999</v>
+      </c>
+      <c r="D15" s="29">
         <f>B15*C15</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+        <v>1.9997999999999998E-2</v>
+      </c>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
       <c r="I15" s="22" t="s">
         <v>63</v>
       </c>
@@ -2392,13 +2390,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+    <row r="16" spans="1:11" ht="72" customHeight="1">
+      <c r="A16" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="15" t="s">
         <v>10</v>
       </c>
@@ -2414,17 +2412,19 @@
       <c r="I16" s="5">
         <v>0.4</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="25">
+        <v>0.33329999999999999</v>
+      </c>
       <c r="K16" s="5">
         <f>I16*J16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+        <v>0.13331999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="51.75">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="15" t="s">
         <v>12</v>
       </c>
@@ -2446,11 +2446,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
+    <row r="18" spans="1:11" ht="45">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="15" t="s">
         <v>13</v>
       </c>
@@ -2472,11 +2472,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
+    <row r="19" spans="1:11" ht="45">
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="15" t="s">
         <v>14</v>
       </c>
@@ -2498,17 +2498,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="40" t="s">
+    <row r="20" spans="1:11">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
       <c r="I20" s="5">
         <f>SUM(I16:I19)</f>
         <v>0.99999999999999989</v>
@@ -2516,28 +2516,28 @@
       <c r="J20" s="25"/>
       <c r="K20" s="5">
         <f>SUM(K16:K19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>0.13331999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="31.5">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="38">
         <v>0.1</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="29">
         <f>K25</f>
         <v>0</v>
       </c>
-      <c r="D21" s="36">
+      <c r="D21" s="29">
         <f>B21*C21</f>
         <v>0</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
       <c r="I21" s="22" t="s">
         <v>63</v>
       </c>
@@ -2548,13 +2548,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:11" ht="51.75">
+      <c r="A22" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="15" t="s">
         <v>18</v>
       </c>
@@ -2576,11 +2576,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+    <row r="23" spans="1:11" ht="51.75">
+      <c r="A23" s="33"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="15" t="s">
         <v>19</v>
       </c>
@@ -2602,11 +2602,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
+    <row r="24" spans="1:11" ht="51.75">
+      <c r="A24" s="33"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="15" t="s">
         <v>20</v>
       </c>
@@ -2628,17 +2628,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="42" t="s">
+    <row r="25" spans="1:11">
+      <c r="A25" s="34"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
       <c r="I25" s="5">
         <f>SUM(I22:I24)</f>
         <v>1</v>
@@ -2649,25 +2649,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="31.5">
       <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="41">
+      <c r="B26" s="38">
         <v>0.2</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="29">
         <f>K30</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="36">
+        <v>0.26663999999999999</v>
+      </c>
+      <c r="D26" s="29">
         <f>B26*C26</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
+        <v>5.3328E-2</v>
+      </c>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
       <c r="I26" s="22" t="s">
         <v>63</v>
       </c>
@@ -2678,13 +2678,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+    <row r="27" spans="1:11" ht="42" customHeight="1">
+      <c r="A27" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="15" t="s">
         <v>22</v>
       </c>
@@ -2700,17 +2700,19 @@
       <c r="I27" s="5">
         <v>0.5</v>
       </c>
-      <c r="J27" s="25"/>
+      <c r="J27" s="25">
+        <v>0.33329999999999999</v>
+      </c>
       <c r="K27" s="5">
         <f>I27*J27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
+        <v>0.16664999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="52">
+      <c r="A28" s="33"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="15" t="s">
         <v>23</v>
       </c>
@@ -2726,17 +2728,19 @@
       <c r="I28" s="5">
         <v>0.3</v>
       </c>
-      <c r="J28" s="25"/>
+      <c r="J28" s="25">
+        <v>0.33329999999999999</v>
+      </c>
       <c r="K28" s="5">
         <f>I28*J28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
+        <v>9.9989999999999996E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="51.75">
+      <c r="A29" s="33"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="15" t="s">
         <v>25</v>
       </c>
@@ -2758,17 +2762,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="40" t="s">
+    <row r="30" spans="1:11">
+      <c r="A30" s="34"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="5">
         <f>SUM(I27:I29)</f>
         <v>1</v>
@@ -2776,28 +2780,28 @@
       <c r="J30" s="25"/>
       <c r="K30" s="5">
         <f>SUM(K27:K29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>0.26663999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="31.5">
       <c r="A31" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="41">
+      <c r="B31" s="38">
         <v>0.05</v>
       </c>
-      <c r="C31" s="36">
+      <c r="C31" s="29">
         <f>K36</f>
         <v>0</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="29">
         <f>B31*C31</f>
         <v>0</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="22" t="s">
         <v>63</v>
       </c>
@@ -2808,13 +2812,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+    <row r="32" spans="1:11" ht="42" customHeight="1">
+      <c r="A32" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="15" t="s">
         <v>28</v>
       </c>
@@ -2836,11 +2840,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
+    <row r="33" spans="1:11" ht="64.5">
+      <c r="A33" s="33"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="15" t="s">
         <v>29</v>
       </c>
@@ -2862,11 +2866,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
+    <row r="34" spans="1:11" ht="64.5">
+      <c r="A34" s="33"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="15" t="s">
         <v>31</v>
       </c>
@@ -2888,11 +2892,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
+    <row r="35" spans="1:11" ht="45">
+      <c r="A35" s="33"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="15" t="s">
         <v>32</v>
       </c>
@@ -2914,17 +2918,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="40" t="s">
+    <row r="36" spans="1:11">
+      <c r="A36" s="34"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
       <c r="I36" s="5">
         <f>SUM(I32:I35)</f>
         <v>1</v>
@@ -2935,25 +2939,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="31.5">
       <c r="A37" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="41">
+      <c r="B37" s="38">
         <v>0.05</v>
       </c>
-      <c r="C37" s="36">
+      <c r="C37" s="29">
         <f>K39</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="36">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="D37" s="29">
         <f>B37*C37</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
+        <v>1.6664999999999999E-2</v>
+      </c>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
       <c r="I37" s="22" t="s">
         <v>63</v>
       </c>
@@ -2964,13 +2968,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
+    <row r="38" spans="1:11" ht="64" customHeight="1">
+      <c r="A38" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
       <c r="E38" s="15" t="s">
         <v>34</v>
       </c>
@@ -2986,23 +2990,25 @@
       <c r="I38" s="5">
         <v>1</v>
       </c>
-      <c r="J38" s="25"/>
+      <c r="J38" s="25">
+        <v>0.33329999999999999</v>
+      </c>
       <c r="K38" s="5">
         <f>I38*J38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="57" t="s">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="42"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="36"/>
       <c r="I39" s="5">
         <f>I38</f>
         <v>1</v>
@@ -3010,10 +3016,10 @@
       <c r="J39" s="25"/>
       <c r="K39" s="5">
         <f>K38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="16" t="s">
         <v>127</v>
       </c>
@@ -3024,7 +3030,7 @@
       <c r="C40" s="2"/>
       <c r="D40" s="1">
         <f>SUM(D2:D39)</f>
-        <v>0</v>
+        <v>0.13331300000000001</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="4"/>
@@ -3033,7 +3039,7 @@
       <c r="I40" s="24"/>
       <c r="J40" s="24"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="6"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -3045,51 +3051,12 @@
       <c r="I41" s="24"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="6"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="P5icd78EoiUsk9YySiovVoCLF6jtJc8F6WafoWntCp/JxKEiNPrphsb5Ym4wZnMicI2e56/Rjqy0GR7g/htv8Q==" saltValue="GtA8uiZn5asKhLdoWtxR9g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="55">
-    <mergeCell ref="D31:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="D15:D20"/>
     <mergeCell ref="E26:H26"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="E31:H31"/>
@@ -3106,6 +3073,45 @@
     <mergeCell ref="E25:H25"/>
     <mergeCell ref="B21:B25"/>
     <mergeCell ref="C21:C25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:C36"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Debe ingresar un número entre 0 y 1" promptTitle="Información" prompt="Sólo se aceptan números entre 0 y 1" sqref="B2:B39">
@@ -3121,7 +3127,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>